<commit_message>
made changes as per reviewer's comments
</commit_message>
<xml_diff>
--- a/Supplementary/Table S6.xlsx
+++ b/Supplementary/Table S6.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Savit/Dropbox/THSTI/Jasneet-Aman paper/Manuscript/V1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savit/Documents/Immunometabolism_MS/Supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD0A0A8-1B42-284A-9487-D9EC147826B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="1" r:id="rId1"/>
     <sheet name="intersecting genes" sheetId="2" r:id="rId2"/>
+    <sheet name="GO terms for PC1, PC2, PC3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="736">
   <si>
     <t>Dim.1</t>
   </si>
@@ -1729,12 +1731,519 @@
   </si>
   <si>
     <t>27 genes that form the intersection of 3 PCs</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>GO term</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>FDR q-value</t>
+  </si>
+  <si>
+    <t>Enrichment (N, B, n, b)</t>
+  </si>
+  <si>
+    <t>GO:0098798</t>
+  </si>
+  <si>
+    <t>mitochondrial protein complex</t>
+  </si>
+  <si>
+    <t>1.48 (1237,240,355,102)</t>
+  </si>
+  <si>
+    <t>GO:0043209</t>
+  </si>
+  <si>
+    <t>myelin sheath</t>
+  </si>
+  <si>
+    <t>1.98 (1237,72,355,41)</t>
+  </si>
+  <si>
+    <t>GO:0098800</t>
+  </si>
+  <si>
+    <t>inner mitochondrial membrane protein complex</t>
+  </si>
+  <si>
+    <t>1.57 (1237,113,355,51)</t>
+  </si>
+  <si>
+    <t>GO:0032991</t>
+  </si>
+  <si>
+    <t>protein-containing complex</t>
+  </si>
+  <si>
+    <t>1.16 (1237,614,355,205)</t>
+  </si>
+  <si>
+    <t>GO:0044422</t>
+  </si>
+  <si>
+    <t>organelle part</t>
+  </si>
+  <si>
+    <t>1.07 (1237,1018,355,312)</t>
+  </si>
+  <si>
+    <t>GO:0050789</t>
+  </si>
+  <si>
+    <t>regulation of biological process</t>
+  </si>
+  <si>
+    <t>1.35 (1237,590,197,127)</t>
+  </si>
+  <si>
+    <t>GO:0019222</t>
+  </si>
+  <si>
+    <t>regulation of metabolic process</t>
+  </si>
+  <si>
+    <t>1.48 (1237,407,197,96)</t>
+  </si>
+  <si>
+    <t>GO:0051716</t>
+  </si>
+  <si>
+    <t>cellular response to stimulus</t>
+  </si>
+  <si>
+    <t>1.61 (1237,296,197,76)</t>
+  </si>
+  <si>
+    <t>GO:0080090</t>
+  </si>
+  <si>
+    <t>regulation of primary metabolic process</t>
+  </si>
+  <si>
+    <t>1.51 (1237,362,197,87)</t>
+  </si>
+  <si>
+    <t>GO:0009893</t>
+  </si>
+  <si>
+    <t>positive regulation of metabolic process</t>
+  </si>
+  <si>
+    <t>1.59 (1237,280,197,71)</t>
+  </si>
+  <si>
+    <t>GO:0050794</t>
+  </si>
+  <si>
+    <t>regulation of cellular process</t>
+  </si>
+  <si>
+    <t>1.34 (1237,554,197,118)</t>
+  </si>
+  <si>
+    <t>GO:0050896</t>
+  </si>
+  <si>
+    <t>response to stimulus</t>
+  </si>
+  <si>
+    <t>1.43 (1237,422,197,96)</t>
+  </si>
+  <si>
+    <t>GO:0051171</t>
+  </si>
+  <si>
+    <t>regulation of nitrogen compound metabolic process</t>
+  </si>
+  <si>
+    <t>1.50 (1237,344,197,82)</t>
+  </si>
+  <si>
+    <t>GO:0010033</t>
+  </si>
+  <si>
+    <t>response to organic substance</t>
+  </si>
+  <si>
+    <t>1.67 (1237,226,197,60)</t>
+  </si>
+  <si>
+    <t>GO:0065007</t>
+  </si>
+  <si>
+    <t>biological regulation</t>
+  </si>
+  <si>
+    <t>1.28 (1237,642,197,131)</t>
+  </si>
+  <si>
+    <t>GO:0042221</t>
+  </si>
+  <si>
+    <t>response to chemical</t>
+  </si>
+  <si>
+    <t>1.54 (1237,294,197,72)</t>
+  </si>
+  <si>
+    <t>GO:0031325</t>
+  </si>
+  <si>
+    <t>positive regulation of cellular metabolic process</t>
+  </si>
+  <si>
+    <t>1.58 (1237,258,197,65)</t>
+  </si>
+  <si>
+    <t>GO:0048518</t>
+  </si>
+  <si>
+    <t>positive regulation of biological process</t>
+  </si>
+  <si>
+    <t>1.42 (1237,403,197,91)</t>
+  </si>
+  <si>
+    <t>GO:0031323</t>
+  </si>
+  <si>
+    <t>regulation of cellular metabolic process</t>
+  </si>
+  <si>
+    <t>1.43 (1237,381,197,87)</t>
+  </si>
+  <si>
+    <t>GO:0060255</t>
+  </si>
+  <si>
+    <t>regulation of macromolecule metabolic process</t>
+  </si>
+  <si>
+    <t>1.48 (1237,326,197,77)</t>
+  </si>
+  <si>
+    <t>GO:0051173</t>
+  </si>
+  <si>
+    <t>positive regulation of nitrogen compound metabolic process</t>
+  </si>
+  <si>
+    <t>1.59 (1237,241,197,61)</t>
+  </si>
+  <si>
+    <t>GO:0048522</t>
+  </si>
+  <si>
+    <t>positive regulation of cellular process</t>
+  </si>
+  <si>
+    <t>1.42 (1237,375,197,85)</t>
+  </si>
+  <si>
+    <t>GO:0010604</t>
+  </si>
+  <si>
+    <t>positive regulation of macromolecule metabolic process</t>
+  </si>
+  <si>
+    <t>1.58 (1237,231,197,58)</t>
+  </si>
+  <si>
+    <t>GO:0070887</t>
+  </si>
+  <si>
+    <t>cellular response to chemical stimulus</t>
+  </si>
+  <si>
+    <t>1.69 (1237,175,197,47)</t>
+  </si>
+  <si>
+    <t>GO:0031347</t>
+  </si>
+  <si>
+    <t>regulation of defense response</t>
+  </si>
+  <si>
+    <t>2.54 (1237,42,197,17)</t>
+  </si>
+  <si>
+    <t>GO:0018209</t>
+  </si>
+  <si>
+    <t>peptidyl-serine modification</t>
+  </si>
+  <si>
+    <t>3.14 (1237,24,197,12)</t>
+  </si>
+  <si>
+    <t>GO:0051247</t>
+  </si>
+  <si>
+    <t>positive regulation of protein metabolic process</t>
+  </si>
+  <si>
+    <t>1.65 (1237,175,197,46)</t>
+  </si>
+  <si>
+    <t>GO:0048523</t>
+  </si>
+  <si>
+    <t>negative regulation of cellular process</t>
+  </si>
+  <si>
+    <t>1.44 (1237,309,197,71)</t>
+  </si>
+  <si>
+    <t>GO:0031324</t>
+  </si>
+  <si>
+    <t>negative regulation of cellular metabolic process</t>
+  </si>
+  <si>
+    <t>1.66 (1237,166,197,44)</t>
+  </si>
+  <si>
+    <t>GO:0050707</t>
+  </si>
+  <si>
+    <t>regulation of cytokine secretion</t>
+  </si>
+  <si>
+    <t>3.49 (1237,18,197,10)</t>
+  </si>
+  <si>
+    <t>GO:0006950</t>
+  </si>
+  <si>
+    <t>response to stress</t>
+  </si>
+  <si>
+    <t>1.45 (1237,299,197,69)</t>
+  </si>
+  <si>
+    <t>GO:0071310</t>
+  </si>
+  <si>
+    <t>cellular response to organic substance</t>
+  </si>
+  <si>
+    <t>1.76 (1237,132,197,37)</t>
+  </si>
+  <si>
+    <t>GO:0006468</t>
+  </si>
+  <si>
+    <t>protein phosphorylation</t>
+  </si>
+  <si>
+    <t>2.40 (1237,47,197,18)</t>
+  </si>
+  <si>
+    <t>GO:0048519</t>
+  </si>
+  <si>
+    <t>negative regulation of biological process</t>
+  </si>
+  <si>
+    <t>1.41 (1237,334,197,75)</t>
+  </si>
+  <si>
+    <t>GO:0051246</t>
+  </si>
+  <si>
+    <t>regulation of protein metabolic process</t>
+  </si>
+  <si>
+    <t>1.50 (1237,247,197,59)</t>
+  </si>
+  <si>
+    <t>GO:0019216</t>
+  </si>
+  <si>
+    <t>regulation of lipid metabolic process</t>
+  </si>
+  <si>
+    <t>2.43 (1237,44,197,17)</t>
+  </si>
+  <si>
+    <t>GO:0018105</t>
+  </si>
+  <si>
+    <t>peptidyl-serine phosphorylation</t>
+  </si>
+  <si>
+    <t>3.14 (1237,22,197,11)</t>
+  </si>
+  <si>
+    <t>GO:0032270</t>
+  </si>
+  <si>
+    <t>positive regulation of cellular protein metabolic process</t>
+  </si>
+  <si>
+    <t>1.65 (1237,164,197,43)</t>
+  </si>
+  <si>
+    <t>GO:0009719</t>
+  </si>
+  <si>
+    <t>response to endogenous stimulus</t>
+  </si>
+  <si>
+    <t>2.01 (1237,78,197,25)</t>
+  </si>
+  <si>
+    <t>GO:0009892</t>
+  </si>
+  <si>
+    <t>negative regulation of metabolic process</t>
+  </si>
+  <si>
+    <t>1.60 (1237,181,197,46)</t>
+  </si>
+  <si>
+    <t>GO:0016310</t>
+  </si>
+  <si>
+    <t>phosphorylation</t>
+  </si>
+  <si>
+    <t>1.89 (1237,93,197,28)</t>
+  </si>
+  <si>
+    <t>GO:0005515</t>
+  </si>
+  <si>
+    <t>protein binding</t>
+  </si>
+  <si>
+    <t>1.37 (1237,591,197,129)</t>
+  </si>
+  <si>
+    <t>GO:0019899</t>
+  </si>
+  <si>
+    <t>enzyme binding</t>
+  </si>
+  <si>
+    <t>1.62 (1237,248,197,64)</t>
+  </si>
+  <si>
+    <t>GO:0005488</t>
+  </si>
+  <si>
+    <t>binding</t>
+  </si>
+  <si>
+    <t>1.18 (1237,873,197,164)</t>
+  </si>
+  <si>
+    <t>GO:0000166</t>
+  </si>
+  <si>
+    <t>nucleotide binding</t>
+  </si>
+  <si>
+    <t>1.42 (1237,313,197,71)</t>
+  </si>
+  <si>
+    <t>GO:0043167</t>
+  </si>
+  <si>
+    <t>ion binding</t>
+  </si>
+  <si>
+    <t>1.29 (1237,495,197,102)</t>
+  </si>
+  <si>
+    <t>GO:0044445</t>
+  </si>
+  <si>
+    <t>cytosolic part</t>
+  </si>
+  <si>
+    <t>3.14 (1237,30,197,15)</t>
+  </si>
+  <si>
+    <t>GO:0005829</t>
+  </si>
+  <si>
+    <t>cytosol</t>
+  </si>
+  <si>
+    <t>1.47 (1237,298,197,70)</t>
+  </si>
+  <si>
+    <t>GO:0005737</t>
+  </si>
+  <si>
+    <t>cytoplasm</t>
+  </si>
+  <si>
+    <t>1.31 (1237,464,197,97)</t>
+  </si>
+  <si>
+    <t>1.24 (1237,590,290,172)</t>
+  </si>
+  <si>
+    <t>1.39 (1237,326,290,106)</t>
+  </si>
+  <si>
+    <t>1.22 (1237,642,290,183)</t>
+  </si>
+  <si>
+    <t>1.25 (1237,554,290,162)</t>
+  </si>
+  <si>
+    <t>1.35 (1237,344,290,109)</t>
+  </si>
+  <si>
+    <t>1.43 (1237,247,290,83)</t>
+  </si>
+  <si>
+    <t>1.33 (1237,362,290,113)</t>
+  </si>
+  <si>
+    <t>1.30 (1237,407,290,124)</t>
+  </si>
+  <si>
+    <t>GO:0030234</t>
+  </si>
+  <si>
+    <t>enzyme regulator activity</t>
+  </si>
+  <si>
+    <t>1.86 (1237,85,290,37)</t>
+  </si>
+  <si>
+    <t>1.21 (1237,591,290,167)</t>
+  </si>
+  <si>
+    <t>GO:0061135</t>
+  </si>
+  <si>
+    <t>endopeptidase regulator activity</t>
+  </si>
+  <si>
+    <t>3.05 (1237,14,290,10)</t>
+  </si>
+  <si>
+    <t>1.31 (1237,464,290,142)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1785,6 +2294,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2052,10 +2564,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G780"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20008,7 +20520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20160,4 +20672,1267 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FD0FF0-3DAD-0E44-A808-7A5138D393B2}">
+  <dimension ref="A1:F62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" t="s">
+        <v>573</v>
+      </c>
+      <c r="C2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.1899999999999999E-7</v>
+      </c>
+      <c r="E2">
+        <v>1.7699999999999999E-4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B3" t="s">
+        <v>576</v>
+      </c>
+      <c r="C3" t="s">
+        <v>577</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.1899999999999999E-7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8.8300000000000005E-5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4" t="s">
+        <v>579</v>
+      </c>
+      <c r="C4" t="s">
+        <v>580</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7.0099999999999996E-5</v>
+      </c>
+      <c r="E4">
+        <v>1.89E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" t="s">
+        <v>582</v>
+      </c>
+      <c r="C5" t="s">
+        <v>583</v>
+      </c>
+      <c r="D5">
+        <v>1.85E-4</v>
+      </c>
+      <c r="E5">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>361</v>
+      </c>
+      <c r="B6" t="s">
+        <v>585</v>
+      </c>
+      <c r="C6" t="s">
+        <v>586</v>
+      </c>
+      <c r="D6">
+        <v>5.3399999999999997E-4</v>
+      </c>
+      <c r="E6">
+        <v>4.7899999999999998E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" t="s">
+        <v>588</v>
+      </c>
+      <c r="C7" t="s">
+        <v>589</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.8900000000000001E-7</v>
+      </c>
+      <c r="E7">
+        <v>1.31E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B8" t="s">
+        <v>591</v>
+      </c>
+      <c r="C8" t="s">
+        <v>592</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.4900000000000001E-7</v>
+      </c>
+      <c r="E8">
+        <v>1.2099999999999999E-3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" t="s">
+        <v>594</v>
+      </c>
+      <c r="C9" t="s">
+        <v>595</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.53E-7</v>
+      </c>
+      <c r="E9">
+        <v>8.1499999999999997E-4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>362</v>
+      </c>
+      <c r="B10" t="s">
+        <v>597</v>
+      </c>
+      <c r="C10" t="s">
+        <v>598</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8.4E-7</v>
+      </c>
+      <c r="E10">
+        <v>1.4499999999999999E-3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B11" t="s">
+        <v>600</v>
+      </c>
+      <c r="C11" t="s">
+        <v>601</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.9400000000000001E-6</v>
+      </c>
+      <c r="E11">
+        <v>2.6900000000000001E-3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" t="s">
+        <v>603</v>
+      </c>
+      <c r="C12" t="s">
+        <v>604</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.5000000000000002E-6</v>
+      </c>
+      <c r="E12">
+        <v>2.8900000000000002E-3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>362</v>
+      </c>
+      <c r="B13" t="s">
+        <v>606</v>
+      </c>
+      <c r="C13" t="s">
+        <v>607</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.6800000000000002E-6</v>
+      </c>
+      <c r="E13">
+        <v>2.65E-3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B14" t="s">
+        <v>609</v>
+      </c>
+      <c r="C14" t="s">
+        <v>610</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.4400000000000001E-6</v>
+      </c>
+      <c r="E14">
+        <v>2.97E-3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B15" t="s">
+        <v>612</v>
+      </c>
+      <c r="C15" t="s">
+        <v>613</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3.4800000000000001E-6</v>
+      </c>
+      <c r="E15">
+        <v>2.6800000000000001E-3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B16" t="s">
+        <v>615</v>
+      </c>
+      <c r="C16" t="s">
+        <v>616</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4.6600000000000003E-6</v>
+      </c>
+      <c r="E16">
+        <v>3.2200000000000002E-3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>362</v>
+      </c>
+      <c r="B17" t="s">
+        <v>618</v>
+      </c>
+      <c r="C17" t="s">
+        <v>619</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="E17">
+        <v>4.4099999999999999E-3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>362</v>
+      </c>
+      <c r="B18" t="s">
+        <v>621</v>
+      </c>
+      <c r="C18" t="s">
+        <v>622</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8.8300000000000002E-6</v>
+      </c>
+      <c r="E18">
+        <v>5.0899999999999999E-3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>362</v>
+      </c>
+      <c r="B19" t="s">
+        <v>624</v>
+      </c>
+      <c r="C19" t="s">
+        <v>625</v>
+      </c>
+      <c r="D19" s="1">
+        <v>9.5400000000000001E-6</v>
+      </c>
+      <c r="E19">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>362</v>
+      </c>
+      <c r="B20" t="s">
+        <v>627</v>
+      </c>
+      <c r="C20" t="s">
+        <v>628</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.08E-5</v>
+      </c>
+      <c r="E20">
+        <v>5.3600000000000002E-3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" t="s">
+        <v>630</v>
+      </c>
+      <c r="C21" t="s">
+        <v>631</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="E21">
+        <v>6.0099999999999997E-3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>362</v>
+      </c>
+      <c r="B22" t="s">
+        <v>633</v>
+      </c>
+      <c r="C22" t="s">
+        <v>634</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.6399999999999999E-5</v>
+      </c>
+      <c r="E22">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>362</v>
+      </c>
+      <c r="B23" t="s">
+        <v>636</v>
+      </c>
+      <c r="C23" t="s">
+        <v>637</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2.1299999999999999E-5</v>
+      </c>
+      <c r="E23">
+        <v>8.6700000000000006E-3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>362</v>
+      </c>
+      <c r="B24" t="s">
+        <v>639</v>
+      </c>
+      <c r="C24" t="s">
+        <v>640</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3.8600000000000003E-5</v>
+      </c>
+      <c r="E24">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>362</v>
+      </c>
+      <c r="B25" t="s">
+        <v>642</v>
+      </c>
+      <c r="C25" t="s">
+        <v>643</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4.2400000000000001E-5</v>
+      </c>
+      <c r="E25">
+        <v>1.54E-2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>362</v>
+      </c>
+      <c r="B26" t="s">
+        <v>645</v>
+      </c>
+      <c r="C26" t="s">
+        <v>646</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8.8700000000000001E-5</v>
+      </c>
+      <c r="E26">
+        <v>3.0700000000000002E-2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>362</v>
+      </c>
+      <c r="B27" t="s">
+        <v>648</v>
+      </c>
+      <c r="C27" t="s">
+        <v>649</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8.9300000000000002E-5</v>
+      </c>
+      <c r="E27">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>362</v>
+      </c>
+      <c r="B28" t="s">
+        <v>651</v>
+      </c>
+      <c r="C28" t="s">
+        <v>652</v>
+      </c>
+      <c r="D28" s="1">
+        <v>9.5799999999999998E-5</v>
+      </c>
+      <c r="E28">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>362</v>
+      </c>
+      <c r="B29" t="s">
+        <v>654</v>
+      </c>
+      <c r="C29" t="s">
+        <v>655</v>
+      </c>
+      <c r="D29">
+        <v>1.03E-4</v>
+      </c>
+      <c r="E29">
+        <v>3.1099999999999999E-2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>362</v>
+      </c>
+      <c r="B30" t="s">
+        <v>657</v>
+      </c>
+      <c r="C30" t="s">
+        <v>658</v>
+      </c>
+      <c r="D30">
+        <v>1.1400000000000001E-4</v>
+      </c>
+      <c r="E30">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>362</v>
+      </c>
+      <c r="B31" t="s">
+        <v>660</v>
+      </c>
+      <c r="C31" t="s">
+        <v>661</v>
+      </c>
+      <c r="D31">
+        <v>1.15E-4</v>
+      </c>
+      <c r="E31">
+        <v>3.1800000000000002E-2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>362</v>
+      </c>
+      <c r="B32" t="s">
+        <v>663</v>
+      </c>
+      <c r="C32" t="s">
+        <v>664</v>
+      </c>
+      <c r="D32">
+        <v>1.18E-4</v>
+      </c>
+      <c r="E32">
+        <v>3.15E-2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>362</v>
+      </c>
+      <c r="B33" t="s">
+        <v>666</v>
+      </c>
+      <c r="C33" t="s">
+        <v>667</v>
+      </c>
+      <c r="D33">
+        <v>1.27E-4</v>
+      </c>
+      <c r="E33">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>362</v>
+      </c>
+      <c r="B34" t="s">
+        <v>669</v>
+      </c>
+      <c r="C34" t="s">
+        <v>670</v>
+      </c>
+      <c r="D34">
+        <v>1.2899999999999999E-4</v>
+      </c>
+      <c r="E34">
+        <v>3.1899999999999998E-2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>362</v>
+      </c>
+      <c r="B35" t="s">
+        <v>672</v>
+      </c>
+      <c r="C35" t="s">
+        <v>673</v>
+      </c>
+      <c r="D35">
+        <v>1.3899999999999999E-4</v>
+      </c>
+      <c r="E35">
+        <v>3.32E-2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>362</v>
+      </c>
+      <c r="B36" t="s">
+        <v>675</v>
+      </c>
+      <c r="C36" t="s">
+        <v>676</v>
+      </c>
+      <c r="D36">
+        <v>1.66E-4</v>
+      </c>
+      <c r="E36">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>362</v>
+      </c>
+      <c r="B37" t="s">
+        <v>678</v>
+      </c>
+      <c r="C37" t="s">
+        <v>679</v>
+      </c>
+      <c r="D37">
+        <v>1.7699999999999999E-4</v>
+      </c>
+      <c r="E37">
+        <v>3.95E-2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>362</v>
+      </c>
+      <c r="B38" t="s">
+        <v>681</v>
+      </c>
+      <c r="C38" t="s">
+        <v>682</v>
+      </c>
+      <c r="D38">
+        <v>1.7899999999999999E-4</v>
+      </c>
+      <c r="E38">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>362</v>
+      </c>
+      <c r="B39" t="s">
+        <v>684</v>
+      </c>
+      <c r="C39" t="s">
+        <v>685</v>
+      </c>
+      <c r="D39">
+        <v>1.85E-4</v>
+      </c>
+      <c r="E39">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>362</v>
+      </c>
+      <c r="B40" t="s">
+        <v>687</v>
+      </c>
+      <c r="C40" t="s">
+        <v>688</v>
+      </c>
+      <c r="D40">
+        <v>1.8900000000000001E-4</v>
+      </c>
+      <c r="E40">
+        <v>3.85E-2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>362</v>
+      </c>
+      <c r="B41" t="s">
+        <v>690</v>
+      </c>
+      <c r="C41" t="s">
+        <v>691</v>
+      </c>
+      <c r="D41">
+        <v>2.3699999999999999E-4</v>
+      </c>
+      <c r="E41">
+        <v>4.6899999999999997E-2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>362</v>
+      </c>
+      <c r="B42" t="s">
+        <v>693</v>
+      </c>
+      <c r="C42" t="s">
+        <v>694</v>
+      </c>
+      <c r="D42">
+        <v>2.5599999999999999E-4</v>
+      </c>
+      <c r="E42">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>362</v>
+      </c>
+      <c r="B43" t="s">
+        <v>696</v>
+      </c>
+      <c r="C43" t="s">
+        <v>697</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3.8999999999999998E-8</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.41E-5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>362</v>
+      </c>
+      <c r="B44" t="s">
+        <v>699</v>
+      </c>
+      <c r="C44" t="s">
+        <v>700</v>
+      </c>
+      <c r="D44" s="1">
+        <v>4.2599999999999999E-6</v>
+      </c>
+      <c r="E44">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>362</v>
+      </c>
+      <c r="B45" t="s">
+        <v>702</v>
+      </c>
+      <c r="C45" t="s">
+        <v>703</v>
+      </c>
+      <c r="D45" s="1">
+        <v>6.8299999999999998E-6</v>
+      </c>
+      <c r="E45">
+        <v>3.7399999999999998E-3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>362</v>
+      </c>
+      <c r="B46" t="s">
+        <v>705</v>
+      </c>
+      <c r="C46" t="s">
+        <v>706</v>
+      </c>
+      <c r="D46">
+        <v>1.65E-4</v>
+      </c>
+      <c r="E46">
+        <v>4.53E-2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>362</v>
+      </c>
+      <c r="B47" t="s">
+        <v>708</v>
+      </c>
+      <c r="C47" t="s">
+        <v>709</v>
+      </c>
+      <c r="D47">
+        <v>1.8100000000000001E-4</v>
+      </c>
+      <c r="E47">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>362</v>
+      </c>
+      <c r="B48" t="s">
+        <v>711</v>
+      </c>
+      <c r="C48" t="s">
+        <v>712</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1.1E-5</v>
+      </c>
+      <c r="E48">
+        <v>8.8800000000000007E-3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>362</v>
+      </c>
+      <c r="B49" t="s">
+        <v>714</v>
+      </c>
+      <c r="C49" t="s">
+        <v>715</v>
+      </c>
+      <c r="D49" s="1">
+        <v>5.2599999999999998E-5</v>
+      </c>
+      <c r="E49">
+        <v>2.12E-2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>362</v>
+      </c>
+      <c r="B50" t="s">
+        <v>717</v>
+      </c>
+      <c r="C50" t="s">
+        <v>718</v>
+      </c>
+      <c r="D50">
+        <v>1.6699999999999999E-4</v>
+      </c>
+      <c r="E50">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>363</v>
+      </c>
+      <c r="B51" t="s">
+        <v>588</v>
+      </c>
+      <c r="C51" t="s">
+        <v>589</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4.0400000000000003E-6</v>
+      </c>
+      <c r="E51">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>363</v>
+      </c>
+      <c r="B52" t="s">
+        <v>630</v>
+      </c>
+      <c r="C52" t="s">
+        <v>631</v>
+      </c>
+      <c r="D52" s="1">
+        <v>7.2799999999999998E-6</v>
+      </c>
+      <c r="E52">
+        <v>2.52E-2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>363</v>
+      </c>
+      <c r="B53" t="s">
+        <v>615</v>
+      </c>
+      <c r="C53" t="s">
+        <v>616</v>
+      </c>
+      <c r="D53" s="1">
+        <v>7.8499999999999994E-6</v>
+      </c>
+      <c r="E53">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>363</v>
+      </c>
+      <c r="B54" t="s">
+        <v>603</v>
+      </c>
+      <c r="C54" t="s">
+        <v>604</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1.03E-5</v>
+      </c>
+      <c r="E54">
+        <v>1.78E-2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>363</v>
+      </c>
+      <c r="B55" t="s">
+        <v>609</v>
+      </c>
+      <c r="C55" t="s">
+        <v>610</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2.1100000000000001E-5</v>
+      </c>
+      <c r="E55">
+        <v>2.92E-2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>363</v>
+      </c>
+      <c r="B56" t="s">
+        <v>675</v>
+      </c>
+      <c r="C56" t="s">
+        <v>676</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2.9799999999999999E-5</v>
+      </c>
+      <c r="E56">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>363</v>
+      </c>
+      <c r="B57" t="s">
+        <v>597</v>
+      </c>
+      <c r="C57" t="s">
+        <v>598</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3.0499999999999999E-5</v>
+      </c>
+      <c r="E57">
+        <v>3.0200000000000001E-2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>363</v>
+      </c>
+      <c r="B58" t="s">
+        <v>591</v>
+      </c>
+      <c r="C58" t="s">
+        <v>592</v>
+      </c>
+      <c r="D58" s="1">
+        <v>3.7499999999999997E-5</v>
+      </c>
+      <c r="E58">
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>363</v>
+      </c>
+      <c r="B59" t="s">
+        <v>728</v>
+      </c>
+      <c r="C59" t="s">
+        <v>729</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1.73E-5</v>
+      </c>
+      <c r="E59">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>363</v>
+      </c>
+      <c r="B60" t="s">
+        <v>696</v>
+      </c>
+      <c r="C60" t="s">
+        <v>697</v>
+      </c>
+      <c r="D60" s="1">
+        <v>8.6100000000000006E-5</v>
+      </c>
+      <c r="E60">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="F60" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>363</v>
+      </c>
+      <c r="B61" t="s">
+        <v>732</v>
+      </c>
+      <c r="C61" t="s">
+        <v>733</v>
+      </c>
+      <c r="D61">
+        <v>1.76E-4</v>
+      </c>
+      <c r="E61">
+        <v>4.82E-2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>363</v>
+      </c>
+      <c r="B62" t="s">
+        <v>717</v>
+      </c>
+      <c r="C62" t="s">
+        <v>718</v>
+      </c>
+      <c r="D62" s="1">
+        <v>3.5099999999999999E-6</v>
+      </c>
+      <c r="E62">
+        <v>2.8300000000000001E-3</v>
+      </c>
+      <c r="F62" t="s">
+        <v>735</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>